<commit_message>
Explosion added and resizing corrected.
</commit_message>
<xml_diff>
--- a/Algs.xlsx
+++ b/Algs.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/v_triputin/AndroidStudioProjects/CradleOfTronesGDX/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DCECA1-C8DA-FA46-9330-0AD6DFDB1DE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,43 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+  <si>
+    <t>Цикл по всем ячейкам</t>
+  </si>
+  <si>
+    <t>Для каждой поиск решений в 4-е стороны</t>
+  </si>
+  <si>
+    <t>Для каждого решения поиск решений</t>
+  </si>
+  <si>
+    <t>Из всех цепочек решений поиск самых длинных</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Cell&gt;</t>
+  </si>
+  <si>
+    <t>Cell parentCell;</t>
+  </si>
+  <si>
+    <t>Cell cell;</t>
+  </si>
+  <si>
+    <t>Итог - arraylist из arraylist &lt;Cells&gt; и какой самый длинный тот и нужен</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +86,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +392,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="40.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Automatic selection logic added. Managed from button.
</commit_message>
<xml_diff>
--- a/Algs.xlsx
+++ b/Algs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/v_triputin/AndroidStudioProjects/CradleOfTronesGDX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DCECA1-C8DA-FA46-9330-0AD6DFDB1DE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DB7011-2CE5-F74C-8C19-909FC44A7F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Цикл по всем ячейкам</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Итог - arraylist из arraylist &lt;Cells&gt; и какой самый длинный тот и нужен</t>
+  </si>
+  <si>
+    <t>Проход по дереву до null и создание arraylist&lt;cells&gt;</t>
+  </si>
+  <si>
+    <t>Рекурсия : на вход массив cells  с текущей cell, наполнение одним из вариантов и вызов рекурсивный .</t>
   </si>
 </sst>
 </file>
@@ -396,12 +402,13 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="40.5" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -472,6 +479,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>8</v>

</xml_diff>